<commit_message>
ajuste no gráfico de barras empilhadas
</commit_message>
<xml_diff>
--- a/_data/out_json/fioce_prodpubl_10.2024.xlsx
+++ b/_data/out_json/fioce_prodpubl_10.2024.xlsx
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F3" t="n">
         <v>9</v>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" t="n">
         <v>25</v>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F8" t="n">
         <v>106</v>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F9" t="n">
         <v>49</v>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F10" t="n">
         <v>7</v>
@@ -714,7 +714,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F11" t="n">
         <v>45</v>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F13" t="n">
         <v>45</v>
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F14" t="n">
         <v>6</v>
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F15" t="n">
         <v>64</v>
@@ -844,7 +844,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F16" t="n">
         <v>23</v>
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F17" t="n">
         <v>69</v>
@@ -896,7 +896,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F18" t="n">
         <v>11</v>
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F19" t="n">
         <v>13</v>
@@ -948,7 +948,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F20" t="n">
         <v>26</v>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F21" t="n">
         <v>74</v>
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F22" t="n">
         <v>110</v>
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F23" t="n">
         <v>31</v>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F24" t="n">
         <v>45</v>
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
@@ -1104,7 +1104,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>89</v>
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F27" t="n">
         <v>21</v>
@@ -1156,7 +1156,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F28" t="n">
         <v>28</v>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>151</v>
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F30" t="n">
         <v>18</v>
@@ -1234,7 +1234,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F31" t="n">
         <v>7</v>
@@ -1260,7 +1260,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F32" t="n">
         <v>45</v>
@@ -1286,7 +1286,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F33" t="n">
         <v>4</v>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F34" t="n">
         <v>42</v>
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>66</v>
@@ -1364,7 +1364,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F36" t="n">
         <v>97</v>
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F37" t="n">
         <v>3</v>
@@ -1416,7 +1416,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F38" t="n">
         <v>55</v>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F39" t="n">
         <v>35</v>
@@ -1468,7 +1468,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F40" t="n">
         <v>6</v>
@@ -1494,7 +1494,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F41" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
Ajuste gráficos de barras por período e boxplots
</commit_message>
<xml_diff>
--- a/_data/out_json/fioce_prodpubl_10.2024.xlsx
+++ b/_data/out_json/fioce_prodpubl_10.2024.xlsx
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F3" t="n">
         <v>9</v>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" t="n">
         <v>25</v>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" t="n">
         <v>106</v>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F9" t="n">
         <v>49</v>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F10" t="n">
         <v>7</v>
@@ -714,7 +714,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F11" t="n">
         <v>45</v>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F13" t="n">
         <v>45</v>
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F14" t="n">
         <v>6</v>
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F15" t="n">
         <v>64</v>
@@ -840,11 +840,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>23</v>
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F17" t="n">
         <v>69</v>
@@ -896,7 +896,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" t="n">
         <v>11</v>
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F19" t="n">
         <v>13</v>
@@ -948,7 +948,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F20" t="n">
         <v>26</v>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F21" t="n">
         <v>74</v>
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F22" t="n">
         <v>110</v>
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" t="n">
         <v>31</v>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F24" t="n">
         <v>45</v>
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
@@ -1104,7 +1104,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>89</v>
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F27" t="n">
         <v>21</v>
@@ -1156,7 +1156,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F28" t="n">
         <v>28</v>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
         <v>151</v>
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F30" t="n">
         <v>18</v>
@@ -1230,11 +1230,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>19/08/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>7</v>
@@ -1260,7 +1260,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F32" t="n">
         <v>45</v>
@@ -1286,7 +1286,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F33" t="n">
         <v>4</v>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F34" t="n">
         <v>42</v>
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
         <v>66</v>
@@ -1364,7 +1364,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F36" t="n">
         <v>97</v>
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F37" t="n">
         <v>3</v>
@@ -1416,7 +1416,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F38" t="n">
         <v>55</v>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F39" t="n">
         <v>35</v>
@@ -1468,7 +1468,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F40" t="n">
         <v>6</v>
@@ -1494,7 +1494,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F41" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
atualização dados pesquisadores fioce
</commit_message>
<xml_diff>
--- a/_data/out_json/fioce_prodpubl_10.2024.xlsx
+++ b/_data/out_json/fioce_prodpubl_10.2024.xlsx
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F3" t="n">
         <v>9</v>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F5" t="n">
         <v>25</v>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F8" t="n">
         <v>106</v>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F9" t="n">
         <v>49</v>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="F10" t="n">
         <v>7</v>
@@ -714,7 +714,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F11" t="n">
         <v>45</v>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F13" t="n">
         <v>45</v>
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F14" t="n">
         <v>6</v>
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F15" t="n">
         <v>64</v>
@@ -844,7 +844,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>23</v>
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F17" t="n">
         <v>69</v>
@@ -896,7 +896,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F18" t="n">
         <v>11</v>
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F19" t="n">
         <v>13</v>
@@ -948,7 +948,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F20" t="n">
         <v>26</v>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F21" t="n">
         <v>74</v>
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F22" t="n">
         <v>110</v>
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F23" t="n">
         <v>31</v>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F24" t="n">
         <v>45</v>
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
@@ -1104,7 +1104,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F26" t="n">
         <v>89</v>
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F27" t="n">
         <v>21</v>
@@ -1156,7 +1156,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F28" t="n">
         <v>28</v>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F29" t="n">
         <v>151</v>
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="F30" t="n">
         <v>18</v>
@@ -1230,14 +1230,14 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -1260,7 +1260,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F32" t="n">
         <v>45</v>
@@ -1286,7 +1286,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="F33" t="n">
         <v>4</v>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F34" t="n">
         <v>42</v>
@@ -1334,14 +1334,14 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36">
@@ -1364,7 +1364,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F36" t="n">
         <v>97</v>
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F37" t="n">
         <v>3</v>
@@ -1416,7 +1416,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F38" t="n">
         <v>55</v>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F39" t="n">
         <v>35</v>
@@ -1468,7 +1468,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F40" t="n">
         <v>6</v>
@@ -1494,7 +1494,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F41" t="n">
         <v>8</v>

</xml_diff>